<commit_message>
all pictures in one table
</commit_message>
<xml_diff>
--- a/0_data/autogen_captions.xlsx
+++ b/0_data/autogen_captions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\network_science\0_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C6D27C-A4AF-4A9A-9B4E-757DE61D9425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA09218-67F8-4D20-B790-26C357B0B068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4606,7 +4606,7 @@
     <t>a picture of a group of beautiful women, dressed in white and purple dresses, pose for a picture one woman wears a white earring and another wears a white and silver earring one woman</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Long</t>
   </si>
 </sst>
 </file>
@@ -4971,8 +4971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B765"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>